<commit_message>
Enviando nova versão (Não solucionou o problema das Beneficiárias)
</commit_message>
<xml_diff>
--- a/BALANÇO_COMPLETO.xlsx
+++ b/BALANÇO_COMPLETO.xlsx
@@ -4150,10 +4150,13 @@
         <f>H16</f>
         <v/>
       </c>
-      <c r="P16" s="25" t="n">
+      <c r="P16" s="25">
+        <f>IF(P15&lt;=0,(N16-O16),P15+(N16-O16))</f>
+        <v/>
+      </c>
+      <c r="Q16" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" s="28" t="n"/>
       <c r="R16" t="inlineStr">
         <is>
           <t>2968374-2</t>

</xml_diff>

<commit_message>
Resolveu o bug de não ler dados com ponto e vírgula (Guilherme)
</commit_message>
<xml_diff>
--- a/BALANÇO_COMPLETO.xlsx
+++ b/BALANÇO_COMPLETO.xlsx
@@ -9,6 +9,7 @@
     <sheet name="RESUMO " sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="UC GERADORA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="UC BENEF. 1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="UC GERADORA 2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1751,12 +1752,12 @@
       </c>
       <c r="F7" s="11" t="inlineStr">
         <is>
-          <t>200027499</t>
+          <t>11641435</t>
         </is>
       </c>
       <c r="G7" s="12" t="inlineStr">
         <is>
-          <t>RUA CARAI, Q. 12, L. 15, S/N PARQUE ITATIAIA</t>
+          <t>ALA JOAO ELIAS DA SILVA CALDAS, Q. 88 A, L. 16, S/N, APART - 1 SETOR PEDRO LUDOVICO</t>
         </is>
       </c>
       <c r="H7" s="158" t="n"/>
@@ -1785,12 +1786,12 @@
       </c>
       <c r="F8" s="8" t="inlineStr">
         <is>
-          <t>10031998761</t>
+          <t>15922595</t>
         </is>
       </c>
       <c r="G8" s="165" t="inlineStr">
         <is>
-          <t>RUA K-4, Q. 01, L. 10, S/N JARDIM ESPLANADA</t>
+          <t>ALA JOAO ELIAS DA SILVA CALDAS, Q. 88 A, L. 16, S/N, - SALA 2 SETOR PEDRO LUDOVICO</t>
         </is>
       </c>
       <c r="H8" s="158" t="n"/>
@@ -2484,12 +2485,12 @@
       </c>
       <c r="B5" s="74" t="inlineStr">
         <is>
-          <t>19/12/2024</t>
+          <t>12/12/2024</t>
         </is>
       </c>
       <c r="C5" s="74" t="inlineStr">
         <is>
-          <t>18/01/2025</t>
+          <t>13/01/2025</t>
         </is>
       </c>
       <c r="D5" s="35">
@@ -2506,13 +2507,13 @@
         <v/>
       </c>
       <c r="I5" s="28" t="n">
-        <v>226</v>
+        <v>1905</v>
       </c>
       <c r="J5" s="28" t="n">
-        <v>181</v>
+        <v>1905</v>
       </c>
       <c r="K5" s="28" t="n">
-        <v>211</v>
+        <v>3947</v>
       </c>
       <c r="L5" s="73">
         <f>(K5+(E5-I5))</f>
@@ -2523,25 +2524,25 @@
         <v/>
       </c>
       <c r="N5" s="180" t="n">
-        <v>27.39</v>
+        <v>2452.62</v>
       </c>
       <c r="O5" s="35">
         <f>I5-J5</f>
         <v/>
       </c>
       <c r="P5" s="28" t="n">
-        <v>1418</v>
+        <v>0</v>
       </c>
       <c r="R5" s="146" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S5" s="146" t="n">
-        <v>16289</v>
+        <v>39429</v>
       </c>
       <c r="T5" s="146" t="n">
-        <v>16500</v>
+        <v>43376</v>
       </c>
     </row>
     <row r="6">
@@ -2552,12 +2553,12 @@
       </c>
       <c r="B6" s="55" t="inlineStr">
         <is>
-          <t>18/01/2025</t>
+          <t>13/01/2025</t>
         </is>
       </c>
       <c r="C6" s="74" t="inlineStr">
         <is>
-          <t>17/02/2025</t>
+          <t>11/02/2025</t>
         </is>
       </c>
       <c r="D6" s="35">
@@ -2571,13 +2572,13 @@
       </c>
       <c r="H6" s="181" t="n"/>
       <c r="I6" s="28" t="n">
-        <v>273</v>
+        <v>1578</v>
       </c>
       <c r="J6" s="28" t="n">
-        <v>160</v>
+        <v>1578</v>
       </c>
       <c r="K6" s="28" t="n">
-        <v>190</v>
+        <v>3520</v>
       </c>
       <c r="L6" s="73">
         <f>(K6+(E6-I6))</f>
@@ -2588,25 +2589,25 @@
         <v/>
       </c>
       <c r="N6" s="180" t="n">
-        <v>34.19</v>
+        <v>2118.4</v>
       </c>
       <c r="O6" s="35">
         <f>I6-J6</f>
         <v/>
       </c>
       <c r="P6" s="28" t="n">
-        <v>1531</v>
+        <v>0</v>
       </c>
       <c r="R6" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S6" s="140" t="n">
-        <v>16500</v>
+        <v>43376</v>
       </c>
       <c r="T6" s="140" t="n">
-        <v>16690</v>
+        <v>46896</v>
       </c>
     </row>
     <row r="7">
@@ -2617,12 +2618,12 @@
       </c>
       <c r="B7" s="55" t="inlineStr">
         <is>
-          <t>17/02/2025</t>
+          <t>11/02/2025</t>
         </is>
       </c>
       <c r="C7" s="74" t="inlineStr">
         <is>
-          <t>19/03/2025</t>
+          <t>12/03/2025</t>
         </is>
       </c>
       <c r="D7" s="35">
@@ -2636,13 +2637,13 @@
       </c>
       <c r="H7" s="181" t="n"/>
       <c r="I7" s="28" t="n">
-        <v>204</v>
+        <v>1725</v>
       </c>
       <c r="J7" s="28" t="n">
-        <v>282</v>
+        <v>1725</v>
       </c>
       <c r="K7" s="28" t="n">
-        <v>312</v>
+        <v>3496</v>
       </c>
       <c r="L7" s="73">
         <f>(K7+(E7-I7))</f>
@@ -2653,25 +2654,25 @@
         <v/>
       </c>
       <c r="N7" s="180" t="n">
-        <v>52.61</v>
+        <v>2048.83</v>
       </c>
       <c r="O7" s="35">
         <f>I7-J7</f>
         <v/>
       </c>
       <c r="P7" s="28" t="n">
-        <v>1453</v>
+        <v>0</v>
       </c>
       <c r="R7" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S7" s="140" t="n">
-        <v>16690</v>
+        <v>46896</v>
       </c>
       <c r="T7" s="140" t="n">
-        <v>17002</v>
+        <v>50392</v>
       </c>
     </row>
     <row r="8">
@@ -2682,12 +2683,12 @@
       </c>
       <c r="B8" s="55" t="inlineStr">
         <is>
-          <t>19/03/2025</t>
+          <t>12/03/2025</t>
         </is>
       </c>
       <c r="C8" s="74" t="inlineStr">
         <is>
-          <t>16/04/2025</t>
+          <t>10/04/2025</t>
         </is>
       </c>
       <c r="D8" s="35">
@@ -2701,13 +2702,13 @@
       </c>
       <c r="H8" s="181" t="n"/>
       <c r="I8" s="28" t="n">
-        <v>155</v>
+        <v>1401</v>
       </c>
       <c r="J8" s="28" t="n">
-        <v>179</v>
+        <v>1401</v>
       </c>
       <c r="K8" s="28" t="n">
-        <v>209</v>
+        <v>3758</v>
       </c>
       <c r="L8" s="73">
         <f>(K8+(E8-I8))</f>
@@ -2718,25 +2719,25 @@
         <v/>
       </c>
       <c r="N8" s="180" t="n">
-        <v>44.52</v>
+        <v>2532.23</v>
       </c>
       <c r="O8" s="35">
         <f>I8-J8</f>
         <v/>
       </c>
       <c r="P8" s="28" t="n">
-        <v>1429</v>
+        <v>0</v>
       </c>
       <c r="R8" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S8" s="140" t="n">
-        <v>17002</v>
+        <v>50392</v>
       </c>
       <c r="T8" s="140" t="n">
-        <v>17211</v>
+        <v>54150</v>
       </c>
     </row>
     <row r="9">
@@ -2747,12 +2748,12 @@
       </c>
       <c r="B9" s="55" t="inlineStr">
         <is>
-          <t>16/04/2025</t>
+          <t>10/04/2025</t>
         </is>
       </c>
       <c r="C9" s="74" t="inlineStr">
         <is>
-          <t>15/05/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="D9" s="35">
@@ -2766,13 +2767,13 @@
       </c>
       <c r="H9" s="181" t="n"/>
       <c r="I9" s="28" t="n">
-        <v>159</v>
+        <v>1501</v>
       </c>
       <c r="J9" s="28" t="n">
-        <v>164</v>
+        <v>2799.23</v>
       </c>
       <c r="K9" s="28" t="n">
-        <v>194</v>
+        <v>3231</v>
       </c>
       <c r="L9" s="73">
         <f>(K9+(E9-I9))</f>
@@ -2783,25 +2784,25 @@
         <v/>
       </c>
       <c r="N9" s="180" t="n">
-        <v>44.77</v>
+        <v>788.2</v>
       </c>
       <c r="O9" s="35">
         <f>I9-J9</f>
         <v/>
       </c>
       <c r="P9" s="28" t="n">
-        <v>1424</v>
+        <v>0</v>
       </c>
       <c r="R9" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S9" s="140" t="n">
-        <v>17211</v>
+        <v>54150</v>
       </c>
       <c r="T9" s="140" t="n">
-        <v>17405</v>
+        <v>57381</v>
       </c>
     </row>
     <row r="10">
@@ -2812,12 +2813,12 @@
       </c>
       <c r="B10" s="55" t="inlineStr">
         <is>
-          <t>15/05/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="C10" s="74" t="inlineStr">
         <is>
-          <t>16/06/2025</t>
+          <t>10/06/2025</t>
         </is>
       </c>
       <c r="D10" s="35">
@@ -2831,13 +2832,13 @@
       </c>
       <c r="H10" s="181" t="n"/>
       <c r="I10" s="28" t="n">
-        <v>154</v>
+        <v>1874</v>
       </c>
       <c r="J10" s="28" t="n">
-        <v>181</v>
+        <v>2947</v>
       </c>
       <c r="K10" s="28" t="n">
-        <v>211</v>
+        <v>2947</v>
       </c>
       <c r="L10" s="73">
         <f>(K10+(E10-I10))</f>
@@ -2848,25 +2849,25 @@
         <v/>
       </c>
       <c r="N10" s="180" t="n">
-        <v>48.03</v>
+        <v>357.36</v>
       </c>
       <c r="O10" s="35">
         <f>I10-J10</f>
         <v/>
       </c>
       <c r="P10" s="28" t="n">
-        <v>1397</v>
+        <v>0</v>
       </c>
       <c r="R10" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S10" s="140" t="n">
-        <v>17405</v>
+        <v>57381</v>
       </c>
       <c r="T10" s="140" t="n">
-        <v>17616</v>
+        <v>60328</v>
       </c>
     </row>
     <row r="11">
@@ -2877,12 +2878,12 @@
       </c>
       <c r="B11" s="55" t="inlineStr">
         <is>
-          <t>16/06/2025</t>
+          <t>10/06/2025</t>
         </is>
       </c>
       <c r="C11" s="74" t="inlineStr">
         <is>
-          <t>18/07/2025</t>
+          <t>12/07/2025</t>
         </is>
       </c>
       <c r="D11" s="35">
@@ -2896,13 +2897,13 @@
       </c>
       <c r="H11" s="181" t="n"/>
       <c r="I11" s="28" t="n">
-        <v>252</v>
+        <v>2589</v>
       </c>
       <c r="J11" s="28" t="n">
-        <v>119</v>
+        <v>2301</v>
       </c>
       <c r="K11" s="28" t="n">
-        <v>149</v>
+        <v>2401</v>
       </c>
       <c r="L11" s="73">
         <f>(K11+(E11-I11))</f>
@@ -2913,25 +2914,25 @@
         <v/>
       </c>
       <c r="N11" s="180" t="n">
-        <v>42.91</v>
+        <v>281.66</v>
       </c>
       <c r="O11" s="35">
         <f>I11-J11</f>
         <v/>
       </c>
       <c r="P11" s="28" t="n">
-        <v>1530</v>
+        <v>906.51</v>
       </c>
       <c r="R11" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S11" s="140" t="n">
-        <v>17616</v>
+        <v>60328</v>
       </c>
       <c r="T11" s="140" t="n">
-        <v>17765</v>
+        <v>62729</v>
       </c>
     </row>
     <row r="12">
@@ -2942,12 +2943,12 @@
       </c>
       <c r="B12" s="55" t="inlineStr">
         <is>
-          <t>18/07/2025</t>
+          <t>12/07/2025</t>
         </is>
       </c>
       <c r="C12" s="74" t="inlineStr">
         <is>
-          <t>18/08/2025</t>
+          <t>11/08/2025</t>
         </is>
       </c>
       <c r="D12" s="35">
@@ -2961,13 +2962,13 @@
       </c>
       <c r="H12" s="181" t="n"/>
       <c r="I12" s="28" t="n">
-        <v>147</v>
+        <v>2700</v>
       </c>
       <c r="J12" s="28" t="n">
-        <v>368</v>
+        <v>1605</v>
       </c>
       <c r="K12" s="28" t="n">
-        <v>398</v>
+        <v>1705</v>
       </c>
       <c r="L12" s="73">
         <f>(K12+(E12-I12))</f>
@@ -2978,25 +2979,25 @@
         <v/>
       </c>
       <c r="N12" s="180" t="n">
-        <v>46.33</v>
+        <v>184.37</v>
       </c>
       <c r="O12" s="35">
         <f>I12-J12</f>
         <v/>
       </c>
       <c r="P12" s="28" t="n">
-        <v>1309</v>
+        <v>2417.78</v>
       </c>
       <c r="R12" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S12" s="140" t="n">
-        <v>17765</v>
+        <v>62729</v>
       </c>
       <c r="T12" s="140" t="n">
-        <v>18163</v>
+        <v>64434</v>
       </c>
     </row>
     <row r="13">
@@ -3007,12 +3008,12 @@
       </c>
       <c r="B13" s="55" t="inlineStr">
         <is>
-          <t>18/08/2025</t>
+          <t>11/08/2025</t>
         </is>
       </c>
       <c r="C13" s="74" t="inlineStr">
         <is>
-          <t>16/09/2025</t>
+          <t>09/09/2025</t>
         </is>
       </c>
       <c r="D13" s="35">
@@ -3026,13 +3027,13 @@
       </c>
       <c r="H13" s="181" t="n"/>
       <c r="I13" s="28" t="n">
-        <v>83</v>
+        <v>2280</v>
       </c>
       <c r="J13" s="28" t="n">
-        <v>511</v>
+        <v>2486.43</v>
       </c>
       <c r="K13" s="28" t="n">
-        <v>541</v>
+        <v>2567</v>
       </c>
       <c r="L13" s="73">
         <f>(K13+(E13-I13))</f>
@@ -3043,25 +3044,25 @@
         <v/>
       </c>
       <c r="N13" s="180" t="n">
-        <v>76.59</v>
+        <v>230.3</v>
       </c>
       <c r="O13" s="35">
         <f>I13-J13</f>
         <v/>
       </c>
       <c r="P13" s="28" t="n">
-        <v>881</v>
+        <v>2417.78</v>
       </c>
       <c r="R13" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S13" s="140" t="n">
-        <v>18163</v>
+        <v>64434</v>
       </c>
       <c r="T13" s="140" t="n">
-        <v>18704</v>
+        <v>67001</v>
       </c>
     </row>
     <row r="14">
@@ -3072,12 +3073,12 @@
       </c>
       <c r="B14" s="55" t="inlineStr">
         <is>
-          <t>16/09/2025</t>
+          <t>09/09/2025</t>
         </is>
       </c>
       <c r="C14" s="74" t="inlineStr">
         <is>
-          <t>16/10/2025</t>
+          <t>10/10/2025</t>
         </is>
       </c>
       <c r="D14" s="35">
@@ -3091,13 +3092,13 @@
       </c>
       <c r="H14" s="181" t="n"/>
       <c r="I14" s="28" t="n">
-        <v>88</v>
+        <v>2510</v>
       </c>
       <c r="J14" s="28" t="n">
-        <v>618</v>
+        <v>3414</v>
       </c>
       <c r="K14" s="28" t="n">
-        <v>648</v>
+        <v>3414</v>
       </c>
       <c r="L14" s="73">
         <f>(K14+(E14-I14))</f>
@@ -3108,25 +3109,25 @@
         <v/>
       </c>
       <c r="N14" s="180" t="n">
-        <v>85.04000000000001</v>
+        <v>385.47</v>
       </c>
       <c r="O14" s="35">
         <f>I14-J14</f>
         <v/>
       </c>
       <c r="P14" s="28" t="n">
-        <v>351</v>
+        <v>2417.78</v>
       </c>
       <c r="R14" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S14" s="140" t="n">
-        <v>18704</v>
+        <v>67001</v>
       </c>
       <c r="T14" s="140" t="n">
-        <v>19352</v>
+        <v>70415</v>
       </c>
     </row>
     <row r="15">
@@ -3137,12 +3138,12 @@
       </c>
       <c r="B15" s="55" t="inlineStr">
         <is>
-          <t>16/10/2025</t>
+          <t>10/10/2025</t>
         </is>
       </c>
       <c r="C15" s="74" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="D15" s="35">
@@ -3156,13 +3157,13 @@
       </c>
       <c r="H15" s="181" t="n"/>
       <c r="I15" s="28" t="n">
-        <v>112</v>
+        <v>2552</v>
       </c>
       <c r="J15" s="28" t="n">
-        <v>463</v>
+        <v>4060</v>
       </c>
       <c r="K15" s="28" t="n">
-        <v>618</v>
+        <v>4060</v>
       </c>
       <c r="L15" s="73">
         <f>(K15+(E15-I15))</f>
@@ -3173,25 +3174,25 @@
         <v/>
       </c>
       <c r="N15" s="180" t="n">
-        <v>248.92</v>
+        <v>498.93</v>
       </c>
       <c r="O15" s="35">
         <f>I15-J15</f>
         <v/>
       </c>
       <c r="P15" s="28" t="n">
-        <v>0</v>
+        <v>2417.78</v>
       </c>
       <c r="R15" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S15" s="140" t="n">
-        <v>19352</v>
+        <v>70415</v>
       </c>
       <c r="T15" s="140" t="n">
-        <v>19970</v>
+        <v>74475</v>
       </c>
     </row>
     <row r="16">
@@ -3202,12 +3203,12 @@
       </c>
       <c r="B16" s="55" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="C16" s="74" t="inlineStr">
         <is>
-          <t>18/12/2025</t>
+          <t>12/12/2025</t>
         </is>
       </c>
       <c r="D16" s="35">
@@ -3221,13 +3222,13 @@
       </c>
       <c r="H16" s="163" t="n"/>
       <c r="I16" s="28" t="n">
-        <v>132</v>
+        <v>2768</v>
       </c>
       <c r="J16" s="28" t="n">
-        <v>132</v>
+        <v>3635</v>
       </c>
       <c r="K16" s="28" t="n">
-        <v>513</v>
+        <v>3635</v>
       </c>
       <c r="L16" s="73">
         <f>(K16+(E16-I16))</f>
@@ -3238,25 +3239,25 @@
         <v/>
       </c>
       <c r="N16" s="180" t="n">
-        <v>511.7</v>
+        <v>456.26</v>
       </c>
       <c r="O16" s="35">
         <f>I16-J16</f>
         <v/>
       </c>
       <c r="P16" s="28" t="n">
-        <v>0</v>
+        <v>1574.38</v>
       </c>
       <c r="R16" s="140" t="inlineStr">
         <is>
-          <t>12378019-5</t>
+          <t>13396929-1</t>
         </is>
       </c>
       <c r="S16" s="140" t="n">
-        <v>19970</v>
+        <v>74475</v>
       </c>
       <c r="T16" s="140" t="n">
-        <v>20483</v>
+        <v>78110</v>
       </c>
     </row>
     <row r="17">
@@ -4082,20 +4083,33 @@
           <t>Nov</t>
         </is>
       </c>
-      <c r="B15" s="55" t="n"/>
-      <c r="C15" s="74" t="n"/>
+      <c r="B15" s="55" t="inlineStr">
+        <is>
+          <t>10/10/2025</t>
+        </is>
+      </c>
+      <c r="C15" s="74" t="inlineStr">
+        <is>
+          <t>11/11/2025</t>
+        </is>
+      </c>
       <c r="E15" s="181" t="n"/>
-      <c r="F15" s="27" t="n"/>
+      <c r="F15" s="27" t="n">
+        <v>1044</v>
+      </c>
       <c r="G15" s="44">
         <f>IFERROR(F15/$E$5,"")</f>
         <v/>
       </c>
-      <c r="H15" s="27" t="n"/>
-      <c r="I15" s="37">
-        <f>IFERROR(H15/F15,"")</f>
-        <v/>
-      </c>
-      <c r="J15" s="180" t="n"/>
+      <c r="H15" s="27" t="n">
+        <v>1044</v>
+      </c>
+      <c r="I15" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="180" t="n">
+        <v>168.17</v>
+      </c>
       <c r="K15" s="47">
         <f>H15-F15</f>
         <v/>
@@ -4116,10 +4130,20 @@
         <f>IF(P14&lt;=0,(N15-O15),P14+(N15-O15))</f>
         <v/>
       </c>
-      <c r="Q15" s="28" t="n"/>
-      <c r="S15" s="140" t="n"/>
-      <c r="T15" s="140" t="n"/>
-      <c r="U15" s="140" t="n"/>
+      <c r="Q15" s="28" t="n">
+        <v>18321.49</v>
+      </c>
+      <c r="S15" s="140" t="inlineStr">
+        <is>
+          <t>12937505-5</t>
+        </is>
+      </c>
+      <c r="T15" s="140" t="n">
+        <v>42129</v>
+      </c>
+      <c r="U15" s="140" t="n">
+        <v>43173</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="122" t="inlineStr">
@@ -4129,30 +4153,30 @@
       </c>
       <c r="B16" s="55" t="inlineStr">
         <is>
-          <t>19/11/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="C16" s="74" t="inlineStr">
         <is>
-          <t>19/12/2025</t>
+          <t>12/12/2025</t>
         </is>
       </c>
       <c r="E16" s="163" t="n"/>
       <c r="F16" s="27" t="n">
-        <v>481</v>
+        <v>1226</v>
       </c>
       <c r="G16" s="44">
         <f>IFERROR(F16/$E$5,"")</f>
         <v/>
       </c>
       <c r="H16" s="27" t="n">
-        <v>0</v>
+        <v>1226</v>
       </c>
       <c r="I16" s="37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="180" t="n">
-        <v>627.24</v>
+        <v>189.75</v>
       </c>
       <c r="K16" s="47">
         <f>H16-F16</f>
@@ -4175,18 +4199,18 @@
         <v/>
       </c>
       <c r="Q16" s="28" t="n">
-        <v>0</v>
+        <v>18777.6</v>
       </c>
       <c r="S16" s="140" t="inlineStr">
         <is>
-          <t>12340952-7</t>
+          <t>12937505-5</t>
         </is>
       </c>
       <c r="T16" s="140" t="n">
-        <v>11694</v>
+        <v>43173</v>
       </c>
       <c r="U16" s="140" t="n">
-        <v>12175</v>
+        <v>44399</v>
       </c>
     </row>
     <row r="17">
@@ -4311,4 +4335,901 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T94"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="11.5546875" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="2.6640625" customWidth="1" min="7" max="7"/>
+    <col width="14.44140625" customWidth="1" min="8" max="8"/>
+    <col width="11.33203125" customWidth="1" min="9" max="9"/>
+    <col width="14.33203125" customWidth="1" min="10" max="10"/>
+    <col width="11.6640625" customWidth="1" min="11" max="11"/>
+    <col width="13.33203125" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="11.6640625" customWidth="1" min="13" max="13"/>
+    <col width="14.5546875" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="16" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="11.5546875" customWidth="1" min="16" max="16"/>
+    <col width="5" customWidth="1" min="17" max="17"/>
+    <col width="15.109375" bestFit="1" customWidth="1" min="18" max="18"/>
+    <col width="13.88671875" customWidth="1" min="19" max="19"/>
+    <col width="15" customWidth="1" min="20" max="20"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="125" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="129" t="inlineStr">
+        <is>
+          <t>UNIDADE GERADORA -</t>
+        </is>
+      </c>
+      <c r="B2" s="173" t="n"/>
+      <c r="C2" s="173" t="n"/>
+      <c r="D2" s="173" t="n"/>
+      <c r="E2" s="173" t="n"/>
+      <c r="F2" s="173" t="n"/>
+      <c r="G2" s="173" t="n"/>
+      <c r="H2" s="173" t="n"/>
+      <c r="I2" s="173" t="n"/>
+      <c r="J2" s="173" t="n"/>
+      <c r="K2" s="174">
+        <f>'RESUMO '!F7</f>
+        <v/>
+      </c>
+      <c r="L2" s="173" t="n"/>
+      <c r="M2" s="173" t="n"/>
+      <c r="N2" s="173" t="n"/>
+      <c r="O2" s="173" t="n"/>
+      <c r="P2" s="158" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="119" t="inlineStr">
+        <is>
+          <t>Mês de Ref.</t>
+        </is>
+      </c>
+      <c r="B3" s="175" t="inlineStr">
+        <is>
+          <t>Período de leitura</t>
+        </is>
+      </c>
+      <c r="C3" s="176" t="n"/>
+      <c r="D3" s="116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geração </t>
+        </is>
+      </c>
+      <c r="E3" s="155" t="n"/>
+      <c r="F3" s="177" t="n"/>
+      <c r="G3" s="121" t="n"/>
+      <c r="H3" s="116" t="inlineStr">
+        <is>
+          <t>Créditos</t>
+        </is>
+      </c>
+      <c r="I3" s="155" t="n"/>
+      <c r="J3" s="155" t="n"/>
+      <c r="K3" s="155" t="n"/>
+      <c r="L3" s="155" t="n"/>
+      <c r="M3" s="155" t="n"/>
+      <c r="N3" s="155" t="n"/>
+      <c r="O3" s="155" t="n"/>
+      <c r="P3" s="177" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="178" t="n"/>
+      <c r="B4" s="141" t="inlineStr">
+        <is>
+          <t>Leitura Anterior</t>
+        </is>
+      </c>
+      <c r="C4" s="142" t="inlineStr">
+        <is>
+          <t>Leitura Atual</t>
+        </is>
+      </c>
+      <c r="D4" s="33" t="inlineStr">
+        <is>
+          <t>Estimativa</t>
+        </is>
+      </c>
+      <c r="E4" s="33" t="inlineStr">
+        <is>
+          <t>Real (Solar View)</t>
+        </is>
+      </c>
+      <c r="F4" s="33" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="H4" s="38" t="inlineStr">
+        <is>
+          <t>Consumo médio</t>
+        </is>
+      </c>
+      <c r="I4" s="48" t="inlineStr">
+        <is>
+          <t>Energia GERAÇÃO</t>
+        </is>
+      </c>
+      <c r="J4" s="48" t="inlineStr">
+        <is>
+          <t>ENREGIA COMPENSADA</t>
+        </is>
+      </c>
+      <c r="K4" s="48" t="inlineStr">
+        <is>
+          <t>ENERGIA ATIVA</t>
+        </is>
+      </c>
+      <c r="L4" s="38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Consumo Real </t>
+        </is>
+      </c>
+      <c r="M4" s="38" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="N4" s="12" t="inlineStr">
+        <is>
+          <t>VALOR FATURA</t>
+        </is>
+      </c>
+      <c r="O4" s="33" t="inlineStr">
+        <is>
+          <t>Mensal (Crédito)</t>
+        </is>
+      </c>
+      <c r="P4" s="48" t="inlineStr">
+        <is>
+          <t>Conferência (Crédito da Fatura) (Olho em saldo na fatura GERADORA, o valor tem que bater com o "Mensal (coluna do lado)" se não tem alguma coisa errada na Equatorial ou na planilha, caso seja na Equatorial, tenho que ligar lá)</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="R4" s="145" t="inlineStr">
+        <is>
+          <t>LEITURA DO MEDIDOR</t>
+        </is>
+      </c>
+      <c r="S4" s="173" t="n"/>
+      <c r="T4" s="158" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="122" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="B5" s="74" t="inlineStr">
+        <is>
+          <t>21/12/2024</t>
+        </is>
+      </c>
+      <c r="C5" s="74" t="inlineStr">
+        <is>
+          <t>21/01/2025</t>
+        </is>
+      </c>
+      <c r="D5" s="35">
+        <f>'RESUMO '!B14</f>
+        <v/>
+      </c>
+      <c r="E5" s="28" t="n"/>
+      <c r="F5" s="34">
+        <f>IFERROR(E5/D5-1,"")</f>
+        <v/>
+      </c>
+      <c r="H5" s="179">
+        <f>'RESUMO '!I7</f>
+        <v/>
+      </c>
+      <c r="I5" s="28" t="n">
+        <v>456</v>
+      </c>
+      <c r="J5" s="28" t="n">
+        <v>436</v>
+      </c>
+      <c r="K5" s="28" t="n">
+        <v>536</v>
+      </c>
+      <c r="L5" s="73">
+        <f>(K5+(E5-I5))</f>
+        <v/>
+      </c>
+      <c r="M5" s="44">
+        <f>IFERROR(L5/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N5" s="180" t="n">
+        <v>154.04</v>
+      </c>
+      <c r="O5" s="35">
+        <f>I5-J5</f>
+        <v/>
+      </c>
+      <c r="P5" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="146" t="inlineStr">
+        <is>
+          <t>13119425-9</t>
+        </is>
+      </c>
+      <c r="S5" s="146" t="n">
+        <v>15604</v>
+      </c>
+      <c r="T5" s="146" t="n">
+        <v>16140</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="122" t="inlineStr">
+        <is>
+          <t>Fev</t>
+        </is>
+      </c>
+      <c r="B6" s="55">
+        <f>C5</f>
+        <v/>
+      </c>
+      <c r="C6" s="74" t="n"/>
+      <c r="D6" s="35">
+        <f>'RESUMO '!B15</f>
+        <v/>
+      </c>
+      <c r="E6" s="28" t="n"/>
+      <c r="F6" s="34">
+        <f>IFERROR(E6/D6-1,"")</f>
+        <v/>
+      </c>
+      <c r="H6" s="181" t="n"/>
+      <c r="I6" s="28" t="n"/>
+      <c r="J6" s="28" t="n"/>
+      <c r="K6" s="28" t="n"/>
+      <c r="L6" s="73">
+        <f>(K6+(E6-I6))</f>
+        <v/>
+      </c>
+      <c r="M6" s="44">
+        <f>IFERROR(L6/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N6" s="180" t="n"/>
+      <c r="O6" s="35">
+        <f>I6-J6</f>
+        <v/>
+      </c>
+      <c r="P6" s="28" t="n"/>
+      <c r="R6" s="140" t="n"/>
+      <c r="S6" s="140" t="n"/>
+      <c r="T6" s="140" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="122" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="B7" s="55">
+        <f>C6</f>
+        <v/>
+      </c>
+      <c r="C7" s="74" t="n"/>
+      <c r="D7" s="35">
+        <f>'RESUMO '!B16</f>
+        <v/>
+      </c>
+      <c r="E7" s="28" t="n"/>
+      <c r="F7" s="34">
+        <f>IFERROR(E7/D7-1,"")</f>
+        <v/>
+      </c>
+      <c r="H7" s="181" t="n"/>
+      <c r="I7" s="28" t="n"/>
+      <c r="J7" s="28" t="n"/>
+      <c r="K7" s="28" t="n"/>
+      <c r="L7" s="73">
+        <f>(K7+(E7-I7))</f>
+        <v/>
+      </c>
+      <c r="M7" s="44">
+        <f>IFERROR(L7/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N7" s="180" t="n"/>
+      <c r="O7" s="35">
+        <f>I7-J7</f>
+        <v/>
+      </c>
+      <c r="P7" s="28" t="n"/>
+      <c r="R7" s="140" t="n"/>
+      <c r="S7" s="140" t="n"/>
+      <c r="T7" s="140" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="122" t="inlineStr">
+        <is>
+          <t>Abr</t>
+        </is>
+      </c>
+      <c r="B8" s="55">
+        <f>C7</f>
+        <v/>
+      </c>
+      <c r="C8" s="74" t="n"/>
+      <c r="D8" s="35">
+        <f>'RESUMO '!B17</f>
+        <v/>
+      </c>
+      <c r="E8" s="28" t="n"/>
+      <c r="F8" s="34">
+        <f>IFERROR(E8/D8-1,"")</f>
+        <v/>
+      </c>
+      <c r="H8" s="181" t="n"/>
+      <c r="I8" s="28" t="n"/>
+      <c r="J8" s="28" t="n"/>
+      <c r="K8" s="28" t="n"/>
+      <c r="L8" s="73">
+        <f>(K8+(E8-I8))</f>
+        <v/>
+      </c>
+      <c r="M8" s="44">
+        <f>IFERROR(L8/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N8" s="180" t="n"/>
+      <c r="O8" s="35">
+        <f>I8-J8</f>
+        <v/>
+      </c>
+      <c r="P8" s="28" t="n"/>
+      <c r="R8" s="140" t="n"/>
+      <c r="S8" s="140" t="n"/>
+      <c r="T8" s="140" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="122" t="inlineStr">
+        <is>
+          <t>Mai</t>
+        </is>
+      </c>
+      <c r="B9" s="55">
+        <f>C8</f>
+        <v/>
+      </c>
+      <c r="C9" s="74" t="n"/>
+      <c r="D9" s="35">
+        <f>'RESUMO '!B18</f>
+        <v/>
+      </c>
+      <c r="E9" s="28" t="n"/>
+      <c r="F9" s="34">
+        <f>IFERROR(E9/D9-1,"")</f>
+        <v/>
+      </c>
+      <c r="H9" s="181" t="n"/>
+      <c r="I9" s="28" t="n"/>
+      <c r="J9" s="28" t="n"/>
+      <c r="K9" s="28" t="n"/>
+      <c r="L9" s="73">
+        <f>(K9+(E9-I9))</f>
+        <v/>
+      </c>
+      <c r="M9" s="44">
+        <f>IFERROR(L9/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N9" s="180" t="n"/>
+      <c r="O9" s="35">
+        <f>I9-J9</f>
+        <v/>
+      </c>
+      <c r="P9" s="28" t="n"/>
+      <c r="R9" s="140" t="n"/>
+      <c r="S9" s="140" t="n"/>
+      <c r="T9" s="140" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="122" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="B10" s="55">
+        <f>C9</f>
+        <v/>
+      </c>
+      <c r="C10" s="74" t="n"/>
+      <c r="D10" s="35">
+        <f>'RESUMO '!B19</f>
+        <v/>
+      </c>
+      <c r="E10" s="28" t="n"/>
+      <c r="F10" s="34">
+        <f>IFERROR(E10/D10-1,"")</f>
+        <v/>
+      </c>
+      <c r="H10" s="181" t="n"/>
+      <c r="I10" s="28" t="n"/>
+      <c r="J10" s="28" t="n"/>
+      <c r="K10" s="28" t="n"/>
+      <c r="L10" s="73">
+        <f>(K10+(E10-I10))</f>
+        <v/>
+      </c>
+      <c r="M10" s="44">
+        <f>IFERROR(L10/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N10" s="180" t="n"/>
+      <c r="O10" s="35">
+        <f>I10-J10</f>
+        <v/>
+      </c>
+      <c r="P10" s="28" t="n"/>
+      <c r="R10" s="140" t="n"/>
+      <c r="S10" s="140" t="n"/>
+      <c r="T10" s="140" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="122" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="B11" s="55">
+        <f>C10</f>
+        <v/>
+      </c>
+      <c r="C11" s="74" t="n"/>
+      <c r="D11" s="35">
+        <f>'RESUMO '!B20</f>
+        <v/>
+      </c>
+      <c r="E11" s="28" t="n"/>
+      <c r="F11" s="34">
+        <f>IFERROR(E11/D11-1,"")</f>
+        <v/>
+      </c>
+      <c r="H11" s="181" t="n"/>
+      <c r="I11" s="28" t="n"/>
+      <c r="J11" s="28" t="n"/>
+      <c r="K11" s="28" t="n"/>
+      <c r="L11" s="73">
+        <f>(K11+(E11-I11))</f>
+        <v/>
+      </c>
+      <c r="M11" s="44">
+        <f>IFERROR(L11/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N11" s="180" t="n"/>
+      <c r="O11" s="35">
+        <f>I11-J11</f>
+        <v/>
+      </c>
+      <c r="P11" s="28" t="n"/>
+      <c r="R11" s="140" t="n"/>
+      <c r="S11" s="140" t="n"/>
+      <c r="T11" s="140" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="122" t="inlineStr">
+        <is>
+          <t>Ago</t>
+        </is>
+      </c>
+      <c r="B12" s="55">
+        <f>C11</f>
+        <v/>
+      </c>
+      <c r="C12" s="74" t="n"/>
+      <c r="D12" s="35">
+        <f>'RESUMO '!B21</f>
+        <v/>
+      </c>
+      <c r="E12" s="28" t="n"/>
+      <c r="F12" s="34">
+        <f>IFERROR(E12/D12-1,"")</f>
+        <v/>
+      </c>
+      <c r="H12" s="181" t="n"/>
+      <c r="I12" s="28" t="n"/>
+      <c r="J12" s="28" t="n"/>
+      <c r="K12" s="28" t="n"/>
+      <c r="L12" s="73">
+        <f>(K12+(E12-I12))</f>
+        <v/>
+      </c>
+      <c r="M12" s="44">
+        <f>IFERROR(L12/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N12" s="180" t="n"/>
+      <c r="O12" s="35">
+        <f>I12-J12</f>
+        <v/>
+      </c>
+      <c r="P12" s="28" t="n"/>
+      <c r="R12" s="140" t="n"/>
+      <c r="S12" s="140" t="n"/>
+      <c r="T12" s="140" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="122" t="inlineStr">
+        <is>
+          <t>Set</t>
+        </is>
+      </c>
+      <c r="B13" s="55">
+        <f>C12</f>
+        <v/>
+      </c>
+      <c r="C13" s="74" t="n"/>
+      <c r="D13" s="35">
+        <f>'RESUMO '!B22</f>
+        <v/>
+      </c>
+      <c r="E13" s="28" t="n"/>
+      <c r="F13" s="34">
+        <f>IFERROR(E13/D13-1,"")</f>
+        <v/>
+      </c>
+      <c r="H13" s="181" t="n"/>
+      <c r="I13" s="28" t="n"/>
+      <c r="J13" s="28" t="n"/>
+      <c r="K13" s="28" t="n"/>
+      <c r="L13" s="73">
+        <f>(K13+(E13-I13))</f>
+        <v/>
+      </c>
+      <c r="M13" s="44">
+        <f>IFERROR(L13/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N13" s="180" t="n"/>
+      <c r="O13" s="35">
+        <f>I13-J13</f>
+        <v/>
+      </c>
+      <c r="P13" s="28" t="n"/>
+      <c r="R13" s="140" t="n"/>
+      <c r="S13" s="140" t="n"/>
+      <c r="T13" s="140" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="122" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="B14" s="55">
+        <f>C13</f>
+        <v/>
+      </c>
+      <c r="C14" s="74" t="n"/>
+      <c r="D14" s="35">
+        <f>'RESUMO '!B23</f>
+        <v/>
+      </c>
+      <c r="E14" s="71" t="n"/>
+      <c r="F14" s="34">
+        <f>IFERROR(E14/D14-1,"")</f>
+        <v/>
+      </c>
+      <c r="H14" s="181" t="n"/>
+      <c r="I14" s="28" t="n"/>
+      <c r="J14" s="28" t="n"/>
+      <c r="K14" s="28" t="n"/>
+      <c r="L14" s="73">
+        <f>(K14+(E14-I14))</f>
+        <v/>
+      </c>
+      <c r="M14" s="44">
+        <f>IFERROR(L14/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N14" s="180" t="n"/>
+      <c r="O14" s="35">
+        <f>I14-J14</f>
+        <v/>
+      </c>
+      <c r="P14" s="28" t="n"/>
+      <c r="R14" s="140" t="n"/>
+      <c r="S14" s="140" t="n"/>
+      <c r="T14" s="140" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="122" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="B15" s="55">
+        <f>C14</f>
+        <v/>
+      </c>
+      <c r="C15" s="74" t="n"/>
+      <c r="D15" s="35">
+        <f>'RESUMO '!B24</f>
+        <v/>
+      </c>
+      <c r="E15" s="28" t="n"/>
+      <c r="F15" s="34">
+        <f>IFERROR(E15/D15-1,"")</f>
+        <v/>
+      </c>
+      <c r="H15" s="181" t="n"/>
+      <c r="I15" s="28" t="n"/>
+      <c r="J15" s="28" t="n"/>
+      <c r="K15" s="28" t="n"/>
+      <c r="L15" s="73">
+        <f>(K15+(E15-I15))</f>
+        <v/>
+      </c>
+      <c r="M15" s="44">
+        <f>IFERROR(L15/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N15" s="180" t="n"/>
+      <c r="O15" s="35">
+        <f>I15-J15</f>
+        <v/>
+      </c>
+      <c r="P15" s="28" t="n"/>
+      <c r="R15" s="140" t="n"/>
+      <c r="S15" s="140" t="n"/>
+      <c r="T15" s="140" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="122" t="inlineStr">
+        <is>
+          <t>Dez</t>
+        </is>
+      </c>
+      <c r="B16" s="55" t="inlineStr">
+        <is>
+          <t>21/11/2025</t>
+        </is>
+      </c>
+      <c r="C16" s="74" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="D16" s="35">
+        <f>'RESUMO '!B25</f>
+        <v/>
+      </c>
+      <c r="E16" s="28" t="n"/>
+      <c r="F16" s="34">
+        <f>IFERROR(E16/D16-1,"")</f>
+        <v/>
+      </c>
+      <c r="H16" s="163" t="n"/>
+      <c r="I16" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="73">
+        <f>(K16+(E16-I16))</f>
+        <v/>
+      </c>
+      <c r="M16" s="44">
+        <f>IFERROR(L16/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N16" s="180" t="n">
+        <v>141.32</v>
+      </c>
+      <c r="O16" s="35">
+        <f>I16-J16</f>
+        <v/>
+      </c>
+      <c r="P16" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="140" t="inlineStr">
+        <is>
+          <t>13119425-9</t>
+        </is>
+      </c>
+      <c r="S16" s="140" t="n">
+        <v>20940</v>
+      </c>
+      <c r="T16" s="140" t="n">
+        <v>21458</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="32" t="inlineStr">
+        <is>
+          <t>∑</t>
+        </is>
+      </c>
+      <c r="B17" s="122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TOTAL </t>
+        </is>
+      </c>
+      <c r="C17" s="158" t="n"/>
+      <c r="D17" s="35">
+        <f>SUM(D5:D16)</f>
+        <v/>
+      </c>
+      <c r="E17" s="35">
+        <f>SUM(E5:E16)</f>
+        <v/>
+      </c>
+      <c r="F17" s="34">
+        <f>IFERROR(E17/D17-1,"")</f>
+        <v/>
+      </c>
+      <c r="H17" s="45">
+        <f>H5*12</f>
+        <v/>
+      </c>
+      <c r="I17" s="35">
+        <f>IFERROR(AVERAGE(I5:I16),"")</f>
+        <v/>
+      </c>
+      <c r="J17" s="35">
+        <f>IFERROR(AVERAGE(J5:J16),"")</f>
+        <v/>
+      </c>
+      <c r="K17" s="35">
+        <f>IFERROR(AVERAGE(K5:K16),"")</f>
+        <v/>
+      </c>
+      <c r="L17" s="35">
+        <f>SUM(L5:L16)</f>
+        <v/>
+      </c>
+      <c r="M17" s="44">
+        <f>IFERROR(L17/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N17" s="31">
+        <f>SUM(N5:N16)</f>
+        <v/>
+      </c>
+      <c r="O17" s="35">
+        <f>SUM(O5:O16)</f>
+        <v/>
+      </c>
+      <c r="P17" s="35">
+        <f>SUM(P5:P16)</f>
+        <v/>
+      </c>
+      <c r="R17" s="140" t="n"/>
+      <c r="S17" s="140" t="n"/>
+      <c r="T17" s="140" t="n"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="122" t="inlineStr">
+        <is>
+          <t>Média =</t>
+        </is>
+      </c>
+      <c r="E18" s="72">
+        <f>AVERAGE(E5:E16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="115" t="inlineStr">
+        <is>
+          <t>LEGENDA</t>
+        </is>
+      </c>
+      <c r="B19" s="173" t="n"/>
+      <c r="C19" s="158" t="n"/>
+      <c r="H19" s="124" t="inlineStr">
+        <is>
+          <t>Obs:. Para Calcular a média de consumo real utilize a forumula -&gt;</t>
+        </is>
+      </c>
+      <c r="L19">
+        <f>AVERAGEIF(L5:L16, "&lt;&gt;0")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>AMARELO</t>
+        </is>
+      </c>
+      <c r="B20" s="21" t="inlineStr">
+        <is>
+          <t>PREENCHER</t>
+        </is>
+      </c>
+      <c r="C20" s="21" t="n"/>
+      <c r="I20" s="123" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="17" t="inlineStr">
+        <is>
+          <t>CINZA</t>
+        </is>
+      </c>
+      <c r="B21" s="22" t="inlineStr">
+        <is>
+          <t>AUTOMÁTICO</t>
+        </is>
+      </c>
+      <c r="C21" s="22" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="36" t="inlineStr">
+        <is>
+          <t>LARANJA</t>
+        </is>
+      </c>
+      <c r="B22" s="182" t="inlineStr">
+        <is>
+          <t>COBRAR</t>
+        </is>
+      </c>
+      <c r="C22" s="158" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="54" t="n"/>
+    </row>
+    <row r="94">
+      <c r="O94" s="1" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="H5:H16"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G3:G17"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H19:K19"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Linha para debuggar código do histórico
</commit_message>
<xml_diff>
--- a/BALANÇO_COMPLETO.xlsx
+++ b/BALANÇO_COMPLETO.xlsx
@@ -20,6 +20,7 @@
     <sheet name="UC BENEF. 10" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="UC BENEF. 11" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="UC BENEF. 12" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="UC GERADORA 2" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -1816,12 +1817,12 @@
       </c>
       <c r="F7" s="11" t="inlineStr">
         <is>
-          <t>10035399889</t>
+          <t>16361337</t>
         </is>
       </c>
       <c r="G7" s="12" t="inlineStr">
         <is>
-          <t>AVENIDA FLORESTA, Q. 46B, L. 05, S/N RESIDENCIAL ALDEIA DO VALE</t>
+          <t>AVENIDA ALPHAVILLE FLAMBOYANT, N. 208 RESIDENCIAL HOUSING FLAMBOYANT</t>
         </is>
       </c>
       <c r="H7" s="161" t="n"/>
@@ -1847,12 +1848,12 @@
       </c>
       <c r="F8" s="8" t="inlineStr">
         <is>
-          <t>10005816643</t>
+          <t>2025003047807</t>
         </is>
       </c>
       <c r="G8" s="168" t="inlineStr">
         <is>
-          <t>RUA DOS BURITIS, Q. 70, L. 5, S/N RESIDENCIAL SANTA FE I</t>
+          <t>AVENIDA CASTELO BRANCO, Q. 38, L. 40, S/N SETOR COIMBRA</t>
         </is>
       </c>
       <c r="H8" s="161" t="n"/>
@@ -1882,8 +1883,16 @@
       <c r="E9" s="105" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="8" t="n"/>
-      <c r="G9" s="168" t="n"/>
+      <c r="F9" s="8" t="inlineStr">
+        <is>
+          <t>11844589</t>
+        </is>
+      </c>
+      <c r="G9" s="168" t="inlineStr">
+        <is>
+          <t>AVENIDA FUED JOSE SEBBA, Q. A 23, L. 12, N. 626, APART - 201, COND - RESID SERRA DOURADA, - - 4 JARDIM GOIAS</t>
+        </is>
+      </c>
       <c r="H9" s="161" t="n"/>
       <c r="I9" s="68" t="n"/>
       <c r="J9" s="4">
@@ -6334,6 +6343,1112 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:T94"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="11.5546875" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="11.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="2.6640625" customWidth="1" min="7" max="7"/>
+    <col width="14.44140625" customWidth="1" min="8" max="8"/>
+    <col width="11.33203125" customWidth="1" min="9" max="9"/>
+    <col width="14.33203125" customWidth="1" min="10" max="10"/>
+    <col width="11.6640625" customWidth="1" min="11" max="11"/>
+    <col width="13.33203125" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="11.6640625" customWidth="1" min="13" max="13"/>
+    <col width="14.5546875" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="16" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="11.5546875" customWidth="1" min="16" max="16"/>
+    <col width="0.6640625" customWidth="1" min="17" max="17"/>
+    <col width="15.109375" bestFit="1" customWidth="1" min="18" max="18"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="122" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="130" t="inlineStr">
+        <is>
+          <t>UNIDADE GERADORA -</t>
+        </is>
+      </c>
+      <c r="B2" s="177" t="n"/>
+      <c r="C2" s="177" t="n"/>
+      <c r="D2" s="177" t="n"/>
+      <c r="E2" s="177" t="n"/>
+      <c r="F2" s="177" t="n"/>
+      <c r="G2" s="177" t="n"/>
+      <c r="H2" s="177" t="n"/>
+      <c r="I2" s="177" t="n"/>
+      <c r="J2" s="177" t="n"/>
+      <c r="K2" s="178">
+        <f>'RESUMO '!F7</f>
+        <v/>
+      </c>
+      <c r="L2" s="177" t="n"/>
+      <c r="M2" s="177" t="n"/>
+      <c r="N2" s="177" t="n"/>
+      <c r="O2" s="177" t="n"/>
+      <c r="P2" s="161" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="116" t="inlineStr">
+        <is>
+          <t>Mês de Ref.</t>
+        </is>
+      </c>
+      <c r="B3" s="123" t="inlineStr">
+        <is>
+          <t>Período de leitura</t>
+        </is>
+      </c>
+      <c r="C3" s="179" t="n"/>
+      <c r="D3" s="113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Geração </t>
+        </is>
+      </c>
+      <c r="E3" s="158" t="n"/>
+      <c r="F3" s="180" t="n"/>
+      <c r="G3" s="118" t="n"/>
+      <c r="H3" s="113" t="inlineStr">
+        <is>
+          <t>Créditos</t>
+        </is>
+      </c>
+      <c r="I3" s="158" t="n"/>
+      <c r="J3" s="158" t="n"/>
+      <c r="K3" s="158" t="n"/>
+      <c r="L3" s="158" t="n"/>
+      <c r="M3" s="158" t="n"/>
+      <c r="N3" s="158" t="n"/>
+      <c r="O3" s="158" t="n"/>
+      <c r="P3" s="180" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="181" t="n"/>
+      <c r="B4" s="182" t="n"/>
+      <c r="C4" s="183" t="n"/>
+      <c r="D4" s="33" t="inlineStr">
+        <is>
+          <t>Estimativa</t>
+        </is>
+      </c>
+      <c r="E4" s="33" t="inlineStr">
+        <is>
+          <t>Real (Solar View)</t>
+        </is>
+      </c>
+      <c r="F4" s="33" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="H4" s="39" t="inlineStr">
+        <is>
+          <t>Consumo médio</t>
+        </is>
+      </c>
+      <c r="I4" s="49" t="inlineStr">
+        <is>
+          <t>E. Injetada (Geração do ultimo ciclo em mensagens importantes na fatura)</t>
+        </is>
+      </c>
+      <c r="J4" s="49" t="inlineStr">
+        <is>
+          <t>E. Compensada (Energia injetada do cliente, se for grupo "A" soma o FP, HR e P em Energia Injetada, em descrição do faturamento)</t>
+        </is>
+      </c>
+      <c r="K4" s="49" t="inlineStr">
+        <is>
+          <t>E. Fornecida (Consumo do cliente, se for grupo "A" soma o FP, HR e P em Energia Ativa Fornecida, em descrição do faturamento)</t>
+        </is>
+      </c>
+      <c r="L4" s="39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Consumo Real </t>
+        </is>
+      </c>
+      <c r="M4" s="39" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="N4" s="12" t="inlineStr">
+        <is>
+          <t>VALOR FATURA</t>
+        </is>
+      </c>
+      <c r="O4" s="33" t="inlineStr">
+        <is>
+          <t>Mensal (Crédito)</t>
+        </is>
+      </c>
+      <c r="P4" s="49" t="inlineStr">
+        <is>
+          <t>Conferência (Crédito da Fatura) (Olho em saldo na fatura GERADORA, o valor tem que bater com o "Mensal (coluna do lado)" se não tem alguma coisa errada na Equatorial ou na planilha, caso seja na Equatorial, tenho que ligar lá)</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="119" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="B5" s="76" t="inlineStr">
+        <is>
+          <t>04/12/2024</t>
+        </is>
+      </c>
+      <c r="C5" s="76" t="inlineStr">
+        <is>
+          <t>03/01/2025</t>
+        </is>
+      </c>
+      <c r="D5" s="35">
+        <f>'RESUMO '!B14</f>
+        <v/>
+      </c>
+      <c r="E5" s="28" t="n"/>
+      <c r="F5" s="34">
+        <f>IFERROR(E5/D5-1,"")</f>
+        <v/>
+      </c>
+      <c r="H5" s="184">
+        <f>'RESUMO '!I7</f>
+        <v/>
+      </c>
+      <c r="I5" s="28" t="n">
+        <v>1353</v>
+      </c>
+      <c r="J5" s="28" t="n">
+        <v>767</v>
+      </c>
+      <c r="K5" s="28" t="n">
+        <v>867</v>
+      </c>
+      <c r="L5" s="75">
+        <f>(K5+(E5-I5))</f>
+        <v/>
+      </c>
+      <c r="M5" s="45">
+        <f>IFERROR(L5/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N5" s="185" t="n">
+        <v>243.85</v>
+      </c>
+      <c r="O5" s="35">
+        <f>I5-J5</f>
+        <v/>
+      </c>
+      <c r="P5" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>35335</v>
+      </c>
+      <c r="T5" t="n">
+        <v>36202</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="119" t="inlineStr">
+        <is>
+          <t>Fev</t>
+        </is>
+      </c>
+      <c r="B6" s="56" t="inlineStr">
+        <is>
+          <t>03/01/2025</t>
+        </is>
+      </c>
+      <c r="C6" s="76" t="inlineStr">
+        <is>
+          <t>04/02/2025</t>
+        </is>
+      </c>
+      <c r="D6" s="35">
+        <f>'RESUMO '!B15</f>
+        <v/>
+      </c>
+      <c r="E6" s="28" t="n"/>
+      <c r="F6" s="34">
+        <f>IFERROR(E6/D6-1,"")</f>
+        <v/>
+      </c>
+      <c r="H6" s="186" t="n"/>
+      <c r="I6" s="28" t="n">
+        <v>1346</v>
+      </c>
+      <c r="J6" s="28" t="n">
+        <v>815</v>
+      </c>
+      <c r="K6" s="28" t="n">
+        <v>915</v>
+      </c>
+      <c r="L6" s="75">
+        <f>(K6+(E6-I6))</f>
+        <v/>
+      </c>
+      <c r="M6" s="45">
+        <f>IFERROR(L6/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N6" s="185" t="n">
+        <v>113.9</v>
+      </c>
+      <c r="O6" s="35">
+        <f>I6-J6</f>
+        <v/>
+      </c>
+      <c r="P6" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>36202</v>
+      </c>
+      <c r="T6" t="n">
+        <v>37117</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="119" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="B7" s="56" t="inlineStr">
+        <is>
+          <t>04/02/2025</t>
+        </is>
+      </c>
+      <c r="C7" s="76" t="inlineStr">
+        <is>
+          <t>05/03/2025</t>
+        </is>
+      </c>
+      <c r="D7" s="35">
+        <f>'RESUMO '!B16</f>
+        <v/>
+      </c>
+      <c r="E7" s="28" t="n"/>
+      <c r="F7" s="34">
+        <f>IFERROR(E7/D7-1,"")</f>
+        <v/>
+      </c>
+      <c r="H7" s="186" t="n"/>
+      <c r="I7" s="28" t="n">
+        <v>1281</v>
+      </c>
+      <c r="J7" s="28" t="n">
+        <v>861</v>
+      </c>
+      <c r="K7" s="28" t="n">
+        <v>961</v>
+      </c>
+      <c r="L7" s="75">
+        <f>(K7+(E7-I7))</f>
+        <v/>
+      </c>
+      <c r="M7" s="45">
+        <f>IFERROR(L7/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N7" s="185" t="n">
+        <v>113.74</v>
+      </c>
+      <c r="O7" s="35">
+        <f>I7-J7</f>
+        <v/>
+      </c>
+      <c r="P7" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>37117</v>
+      </c>
+      <c r="T7" t="n">
+        <v>38078</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="119" t="inlineStr">
+        <is>
+          <t>Abr</t>
+        </is>
+      </c>
+      <c r="B8" s="56" t="inlineStr">
+        <is>
+          <t>05/03/2025</t>
+        </is>
+      </c>
+      <c r="C8" s="76" t="inlineStr">
+        <is>
+          <t>02/04/2025</t>
+        </is>
+      </c>
+      <c r="D8" s="35">
+        <f>'RESUMO '!B17</f>
+        <v/>
+      </c>
+      <c r="E8" s="28" t="n"/>
+      <c r="F8" s="34">
+        <f>IFERROR(E8/D8-1,"")</f>
+        <v/>
+      </c>
+      <c r="H8" s="186" t="n"/>
+      <c r="I8" s="28" t="n">
+        <v>1004</v>
+      </c>
+      <c r="J8" s="28" t="n">
+        <v>941</v>
+      </c>
+      <c r="K8" s="28" t="n">
+        <v>1041</v>
+      </c>
+      <c r="L8" s="75">
+        <f>(K8+(E8-I8))</f>
+        <v/>
+      </c>
+      <c r="M8" s="45">
+        <f>IFERROR(L8/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N8" s="185" t="n">
+        <v>118.77</v>
+      </c>
+      <c r="O8" s="35">
+        <f>I8-J8</f>
+        <v/>
+      </c>
+      <c r="P8" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>38078</v>
+      </c>
+      <c r="T8" t="n">
+        <v>39119</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="119" t="inlineStr">
+        <is>
+          <t>Mai</t>
+        </is>
+      </c>
+      <c r="B9" s="56" t="inlineStr">
+        <is>
+          <t>02/04/2025</t>
+        </is>
+      </c>
+      <c r="C9" s="76" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="D9" s="35">
+        <f>'RESUMO '!B18</f>
+        <v/>
+      </c>
+      <c r="E9" s="28" t="n"/>
+      <c r="F9" s="34">
+        <f>IFERROR(E9/D9-1,"")</f>
+        <v/>
+      </c>
+      <c r="H9" s="186" t="n"/>
+      <c r="I9" s="28" t="n">
+        <v>964</v>
+      </c>
+      <c r="J9" s="28" t="n">
+        <v>869</v>
+      </c>
+      <c r="K9" s="28" t="n">
+        <v>969</v>
+      </c>
+      <c r="L9" s="75">
+        <f>(K9+(E9-I9))</f>
+        <v/>
+      </c>
+      <c r="M9" s="45">
+        <f>IFERROR(L9/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N9" s="185" t="n">
+        <v>110.24</v>
+      </c>
+      <c r="O9" s="35">
+        <f>I9-J9</f>
+        <v/>
+      </c>
+      <c r="P9" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>39119</v>
+      </c>
+      <c r="T9" t="n">
+        <v>40088</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="119" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="B10" s="56" t="inlineStr">
+        <is>
+          <t>02/05/2025</t>
+        </is>
+      </c>
+      <c r="C10" s="76" t="inlineStr">
+        <is>
+          <t>03/06/2025</t>
+        </is>
+      </c>
+      <c r="D10" s="35">
+        <f>'RESUMO '!B19</f>
+        <v/>
+      </c>
+      <c r="E10" s="28" t="n"/>
+      <c r="F10" s="34">
+        <f>IFERROR(E10/D10-1,"")</f>
+        <v/>
+      </c>
+      <c r="H10" s="186" t="n"/>
+      <c r="I10" s="28" t="n">
+        <v>1025</v>
+      </c>
+      <c r="J10" s="28" t="n">
+        <v>815</v>
+      </c>
+      <c r="K10" s="28" t="n">
+        <v>915</v>
+      </c>
+      <c r="L10" s="75">
+        <f>(K10+(E10-I10))</f>
+        <v/>
+      </c>
+      <c r="M10" s="45">
+        <f>IFERROR(L10/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N10" s="185" t="n">
+        <v>115.08</v>
+      </c>
+      <c r="O10" s="35">
+        <f>I10-J10</f>
+        <v/>
+      </c>
+      <c r="P10" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>40088</v>
+      </c>
+      <c r="T10" t="n">
+        <v>41003</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="119" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="B11" s="56" t="inlineStr">
+        <is>
+          <t>03/06/2025</t>
+        </is>
+      </c>
+      <c r="C11" s="76" t="inlineStr">
+        <is>
+          <t>05/07/2025</t>
+        </is>
+      </c>
+      <c r="D11" s="35">
+        <f>'RESUMO '!B20</f>
+        <v/>
+      </c>
+      <c r="E11" s="28" t="n"/>
+      <c r="F11" s="34">
+        <f>IFERROR(E11/D11-1,"")</f>
+        <v/>
+      </c>
+      <c r="H11" s="186" t="n"/>
+      <c r="I11" s="28" t="n">
+        <v>871</v>
+      </c>
+      <c r="J11" s="28" t="n">
+        <v>814</v>
+      </c>
+      <c r="K11" s="28" t="n">
+        <v>914</v>
+      </c>
+      <c r="L11" s="75">
+        <f>(K11+(E11-I11))</f>
+        <v/>
+      </c>
+      <c r="M11" s="45">
+        <f>IFERROR(L11/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N11" s="185" t="n">
+        <v>115.11</v>
+      </c>
+      <c r="O11" s="35">
+        <f>I11-J11</f>
+        <v/>
+      </c>
+      <c r="P11" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
+        <v>41003</v>
+      </c>
+      <c r="T11" t="n">
+        <v>41917</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="119" t="inlineStr">
+        <is>
+          <t>Ago</t>
+        </is>
+      </c>
+      <c r="B12" s="56" t="inlineStr">
+        <is>
+          <t>05/07/2025</t>
+        </is>
+      </c>
+      <c r="C12" s="76" t="inlineStr">
+        <is>
+          <t>02/08/2025</t>
+        </is>
+      </c>
+      <c r="D12" s="35">
+        <f>'RESUMO '!B21</f>
+        <v/>
+      </c>
+      <c r="E12" s="28" t="n"/>
+      <c r="F12" s="34">
+        <f>IFERROR(E12/D12-1,"")</f>
+        <v/>
+      </c>
+      <c r="H12" s="186" t="n"/>
+      <c r="I12" s="28" t="n">
+        <v>718</v>
+      </c>
+      <c r="J12" s="28" t="n">
+        <v>718</v>
+      </c>
+      <c r="K12" s="28" t="n">
+        <v>873</v>
+      </c>
+      <c r="L12" s="75">
+        <f>(K12+(E12-I12))</f>
+        <v/>
+      </c>
+      <c r="M12" s="45">
+        <f>IFERROR(L12/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N12" s="185" t="n">
+        <v>174.2</v>
+      </c>
+      <c r="O12" s="35">
+        <f>I12-J12</f>
+        <v/>
+      </c>
+      <c r="P12" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
+        <v>41917</v>
+      </c>
+      <c r="T12" t="n">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="119" t="inlineStr">
+        <is>
+          <t>Set</t>
+        </is>
+      </c>
+      <c r="B13" s="56" t="inlineStr">
+        <is>
+          <t>02/08/2025</t>
+        </is>
+      </c>
+      <c r="C13" s="76" t="inlineStr">
+        <is>
+          <t>02/09/2025</t>
+        </is>
+      </c>
+      <c r="D13" s="35">
+        <f>'RESUMO '!B22</f>
+        <v/>
+      </c>
+      <c r="E13" s="28" t="n"/>
+      <c r="F13" s="34">
+        <f>IFERROR(E13/D13-1,"")</f>
+        <v/>
+      </c>
+      <c r="H13" s="186" t="n"/>
+      <c r="I13" s="28" t="n">
+        <v>748</v>
+      </c>
+      <c r="J13" s="28" t="n">
+        <v>748</v>
+      </c>
+      <c r="K13" s="28" t="n">
+        <v>990</v>
+      </c>
+      <c r="L13" s="75">
+        <f>(K13+(E13-I13))</f>
+        <v/>
+      </c>
+      <c r="M13" s="45">
+        <f>IFERROR(L13/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N13" s="185" t="n">
+        <v>271.68</v>
+      </c>
+      <c r="O13" s="35">
+        <f>I13-J13</f>
+        <v/>
+      </c>
+      <c r="P13" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S13" t="n">
+        <v>42790</v>
+      </c>
+      <c r="T13" t="n">
+        <v>43780</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="119" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="B14" s="56" t="inlineStr">
+        <is>
+          <t>02/09/2025</t>
+        </is>
+      </c>
+      <c r="C14" s="76" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="D14" s="35">
+        <f>'RESUMO '!B23</f>
+        <v/>
+      </c>
+      <c r="E14" s="73" t="n"/>
+      <c r="F14" s="34">
+        <f>IFERROR(E14/D14-1,"")</f>
+        <v/>
+      </c>
+      <c r="H14" s="186" t="n"/>
+      <c r="I14" s="28" t="n">
+        <v>899</v>
+      </c>
+      <c r="J14" s="28" t="n">
+        <v>899</v>
+      </c>
+      <c r="K14" s="28" t="n">
+        <v>1083</v>
+      </c>
+      <c r="L14" s="75">
+        <f>(K14+(E14-I14))</f>
+        <v/>
+      </c>
+      <c r="M14" s="45">
+        <f>IFERROR(L14/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N14" s="185" t="n">
+        <v>233.85</v>
+      </c>
+      <c r="O14" s="35">
+        <f>I14-J14</f>
+        <v/>
+      </c>
+      <c r="P14" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S14" t="n">
+        <v>43780</v>
+      </c>
+      <c r="T14" t="n">
+        <v>44863</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="119" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="B15" s="56" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="C15" s="76" t="inlineStr">
+        <is>
+          <t>03/11/2025</t>
+        </is>
+      </c>
+      <c r="D15" s="35">
+        <f>'RESUMO '!B24</f>
+        <v/>
+      </c>
+      <c r="E15" s="28" t="n"/>
+      <c r="F15" s="34">
+        <f>IFERROR(E15/D15-1,"")</f>
+        <v/>
+      </c>
+      <c r="H15" s="186" t="n"/>
+      <c r="I15" s="28" t="n">
+        <v>1071</v>
+      </c>
+      <c r="J15" s="28" t="n">
+        <v>1071</v>
+      </c>
+      <c r="K15" s="28" t="n">
+        <v>1259</v>
+      </c>
+      <c r="L15" s="75">
+        <f>(K15+(E15-I15))</f>
+        <v/>
+      </c>
+      <c r="M15" s="45">
+        <f>IFERROR(L15/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N15" s="185" t="n">
+        <v>234.97</v>
+      </c>
+      <c r="O15" s="35">
+        <f>I15-J15</f>
+        <v/>
+      </c>
+      <c r="P15" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
+        <v>44863</v>
+      </c>
+      <c r="T15" t="n">
+        <v>46122</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="119" t="inlineStr">
+        <is>
+          <t>Dez</t>
+        </is>
+      </c>
+      <c r="B16" s="56" t="inlineStr">
+        <is>
+          <t>03/11/2025</t>
+        </is>
+      </c>
+      <c r="C16" s="76" t="inlineStr">
+        <is>
+          <t>05/12/2025</t>
+        </is>
+      </c>
+      <c r="D16" s="35">
+        <f>'RESUMO '!B25</f>
+        <v/>
+      </c>
+      <c r="E16" s="28" t="n"/>
+      <c r="F16" s="34">
+        <f>IFERROR(E16/D16-1,"")</f>
+        <v/>
+      </c>
+      <c r="H16" s="166" t="n"/>
+      <c r="I16" s="28" t="n">
+        <v>302</v>
+      </c>
+      <c r="J16" s="28" t="n">
+        <v>302</v>
+      </c>
+      <c r="K16" s="28" t="n">
+        <v>2051</v>
+      </c>
+      <c r="L16" s="75">
+        <f>(K16+(E16-I16))</f>
+        <v/>
+      </c>
+      <c r="M16" s="45">
+        <f>IFERROR(L16/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N16" s="185" t="n">
+        <v>2161.85</v>
+      </c>
+      <c r="O16" s="35">
+        <f>I16-J16</f>
+        <v/>
+      </c>
+      <c r="P16" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>12774111-9</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>46122</v>
+      </c>
+      <c r="T16" t="n">
+        <v>48173</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="32" t="inlineStr">
+        <is>
+          <t>∑</t>
+        </is>
+      </c>
+      <c r="B17" s="119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">TOTAL </t>
+        </is>
+      </c>
+      <c r="C17" s="161" t="n"/>
+      <c r="D17" s="35">
+        <f>SUM(D5:D16)</f>
+        <v/>
+      </c>
+      <c r="E17" s="35">
+        <f>SUM(E5:E16)</f>
+        <v/>
+      </c>
+      <c r="F17" s="34">
+        <f>IFERROR(E17/D17-1,"")</f>
+        <v/>
+      </c>
+      <c r="H17" s="46">
+        <f>H5*12</f>
+        <v/>
+      </c>
+      <c r="I17" s="35">
+        <f>IFERROR(AVERAGE(I5:I16),"")</f>
+        <v/>
+      </c>
+      <c r="J17" s="35">
+        <f>IFERROR(AVERAGE(J5:J16),"")</f>
+        <v/>
+      </c>
+      <c r="K17" s="35">
+        <f>IFERROR(AVERAGE(K5:K16),"")</f>
+        <v/>
+      </c>
+      <c r="L17" s="35">
+        <f>SUM(L5:L16)</f>
+        <v/>
+      </c>
+      <c r="M17" s="45">
+        <f>IFERROR(L17/$H$5,"")</f>
+        <v/>
+      </c>
+      <c r="N17" s="31">
+        <f>SUM(N5:N16)</f>
+        <v/>
+      </c>
+      <c r="O17" s="35">
+        <f>SUM(O5:O16)</f>
+        <v/>
+      </c>
+      <c r="P17" s="35">
+        <f>SUM(P5:P16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="119" t="inlineStr">
+        <is>
+          <t>Média =</t>
+        </is>
+      </c>
+      <c r="E18" s="74">
+        <f>AVERAGE(E5:E16)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="112" t="inlineStr">
+        <is>
+          <t>LEGENDA</t>
+        </is>
+      </c>
+      <c r="B19" s="177" t="n"/>
+      <c r="C19" s="161" t="n"/>
+      <c r="H19" s="121" t="inlineStr">
+        <is>
+          <t>Obs:. Para Calcular a média de consumo real utilize a forumula -&gt;</t>
+        </is>
+      </c>
+      <c r="L19">
+        <f>AVERAGEIF(L5:L16, "&lt;&gt;0")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>AMARELO</t>
+        </is>
+      </c>
+      <c r="B20" s="21" t="inlineStr">
+        <is>
+          <t>PREENCHER</t>
+        </is>
+      </c>
+      <c r="C20" s="21" t="n"/>
+      <c r="I20" s="120" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="17" t="inlineStr">
+        <is>
+          <t>CINZA</t>
+        </is>
+      </c>
+      <c r="B21" s="22" t="inlineStr">
+        <is>
+          <t>AUTOMÁTICO</t>
+        </is>
+      </c>
+      <c r="C21" s="22" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="36" t="inlineStr">
+        <is>
+          <t>LARANJA</t>
+        </is>
+      </c>
+      <c r="B22" s="187" t="inlineStr">
+        <is>
+          <t>COBRAR</t>
+        </is>
+      </c>
+      <c r="C22" s="161" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="55" t="n"/>
+    </row>
+    <row r="94">
+      <c r="O94" s="1" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="H5:H16"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G3:G17"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="H3:P3"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H19:K19"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -6507,12 +7622,12 @@
       </c>
       <c r="B5" s="76" t="inlineStr">
         <is>
-          <t>26/12/2024</t>
+          <t>27/12/2024</t>
         </is>
       </c>
       <c r="C5" s="76" t="inlineStr">
         <is>
-          <t>24/01/2025</t>
+          <t>27/01/2025</t>
         </is>
       </c>
       <c r="D5" s="35">
@@ -6529,13 +7644,13 @@
         <v/>
       </c>
       <c r="I5" s="28" t="n">
-        <v>1</v>
+        <v>829</v>
       </c>
       <c r="J5" s="28" t="n">
-        <v>437</v>
+        <v>845</v>
       </c>
       <c r="K5" s="28" t="n">
-        <v>537</v>
+        <v>945</v>
       </c>
       <c r="L5" s="75">
         <f>(K5+(E5-I5))</f>
@@ -6546,25 +7661,25 @@
         <v/>
       </c>
       <c r="N5" s="185" t="n">
-        <v>152.02</v>
+        <v>103.93</v>
       </c>
       <c r="O5" s="35">
         <f>I5-J5</f>
         <v/>
       </c>
       <c r="P5" s="28" t="n">
-        <v>1521.25</v>
+        <v>277</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S5" t="n">
-        <v>10916</v>
+        <v>20836</v>
       </c>
       <c r="T5" t="n">
-        <v>11453</v>
+        <v>21781</v>
       </c>
     </row>
     <row r="6">
@@ -6575,12 +7690,12 @@
       </c>
       <c r="B6" s="56" t="inlineStr">
         <is>
-          <t>24/01/2025</t>
+          <t>27/01/2025</t>
         </is>
       </c>
       <c r="C6" s="76" t="inlineStr">
         <is>
-          <t>24/02/2025</t>
+          <t>25/02/2025</t>
         </is>
       </c>
       <c r="D6" s="35">
@@ -6594,13 +7709,13 @@
       </c>
       <c r="H6" s="186" t="n"/>
       <c r="I6" s="28" t="n">
-        <v>1</v>
+        <v>825</v>
       </c>
       <c r="J6" s="28" t="n">
-        <v>797</v>
+        <v>685</v>
       </c>
       <c r="K6" s="28" t="n">
-        <v>897</v>
+        <v>785</v>
       </c>
       <c r="L6" s="75">
         <f>(K6+(E6-I6))</f>
@@ -6611,25 +7726,25 @@
         <v/>
       </c>
       <c r="N6" s="185" t="n">
-        <v>98.09</v>
+        <v>0</v>
       </c>
       <c r="O6" s="35">
         <f>I6-J6</f>
         <v/>
       </c>
       <c r="P6" s="28" t="n">
-        <v>1785.85</v>
+        <v>542.5</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S6" t="n">
-        <v>11453</v>
+        <v>21781</v>
       </c>
       <c r="T6" t="n">
-        <v>12350</v>
+        <v>22566</v>
       </c>
     </row>
     <row r="7">
@@ -6638,16 +7753,11 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="B7" s="56" t="inlineStr">
-        <is>
-          <t>24/02/2025</t>
-        </is>
-      </c>
-      <c r="C7" s="76" t="inlineStr">
-        <is>
-          <t>26/03/2025</t>
-        </is>
-      </c>
+      <c r="B7" s="56">
+        <f>C6</f>
+        <v/>
+      </c>
+      <c r="C7" s="76" t="n"/>
       <c r="D7" s="35">
         <f>'RESUMO '!B16</f>
         <v/>
@@ -6658,15 +7768,9 @@
         <v/>
       </c>
       <c r="H7" s="186" t="n"/>
-      <c r="I7" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="28" t="n">
-        <v>778</v>
-      </c>
-      <c r="K7" s="28" t="n">
-        <v>878</v>
-      </c>
+      <c r="I7" s="28" t="n"/>
+      <c r="J7" s="28" t="n"/>
+      <c r="K7" s="28" t="n"/>
       <c r="L7" s="75">
         <f>(K7+(E7-I7))</f>
         <v/>
@@ -6675,27 +7779,12 @@
         <f>IFERROR(L7/$H$5,"")</f>
         <v/>
       </c>
-      <c r="N7" s="185" t="n">
-        <v>113.74</v>
-      </c>
+      <c r="N7" s="185" t="n"/>
       <c r="O7" s="35">
         <f>I7-J7</f>
         <v/>
       </c>
-      <c r="P7" s="28" t="n">
-        <v>2183.85</v>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>12932377-2</t>
-        </is>
-      </c>
-      <c r="S7" t="n">
-        <v>12350</v>
-      </c>
-      <c r="T7" t="n">
-        <v>13228</v>
-      </c>
+      <c r="P7" s="28" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="119" t="inlineStr">
@@ -6705,12 +7794,12 @@
       </c>
       <c r="B8" s="56" t="inlineStr">
         <is>
-          <t>26/03/2025</t>
+          <t>27/03/2025</t>
         </is>
       </c>
       <c r="C8" s="76" t="inlineStr">
         <is>
-          <t>25/04/2025</t>
+          <t>26/04/2025</t>
         </is>
       </c>
       <c r="D8" s="35">
@@ -6724,13 +7813,13 @@
       </c>
       <c r="H8" s="186" t="n"/>
       <c r="I8" s="28" t="n">
-        <v>1</v>
+        <v>697</v>
       </c>
       <c r="J8" s="28" t="n">
-        <v>1059</v>
+        <v>887</v>
       </c>
       <c r="K8" s="28" t="n">
-        <v>1159</v>
+        <v>987</v>
       </c>
       <c r="L8" s="75">
         <f>(K8+(E8-I8))</f>
@@ -6741,25 +7830,25 @@
         <v/>
       </c>
       <c r="N8" s="185" t="n">
-        <v>105.13</v>
+        <v>113.45</v>
       </c>
       <c r="O8" s="35">
         <f>I8-J8</f>
         <v/>
       </c>
       <c r="P8" s="28" t="n">
-        <v>2152.05</v>
+        <v>594</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S8" t="n">
-        <v>13228</v>
+        <v>23377</v>
       </c>
       <c r="T8" t="n">
-        <v>14387</v>
+        <v>24364</v>
       </c>
     </row>
     <row r="9">
@@ -6770,12 +7859,12 @@
       </c>
       <c r="B9" s="56" t="inlineStr">
         <is>
-          <t>25/04/2025</t>
+          <t>26/04/2025</t>
         </is>
       </c>
       <c r="C9" s="76" t="inlineStr">
         <is>
-          <t>27/05/2025</t>
+          <t>28/05/2025</t>
         </is>
       </c>
       <c r="D9" s="35">
@@ -6789,13 +7878,13 @@
       </c>
       <c r="H9" s="186" t="n"/>
       <c r="I9" s="28" t="n">
-        <v>1</v>
+        <v>766</v>
       </c>
       <c r="J9" s="28" t="n">
-        <v>2121</v>
+        <v>885</v>
       </c>
       <c r="K9" s="28" t="n">
-        <v>2221</v>
+        <v>985</v>
       </c>
       <c r="L9" s="75">
         <f>(K9+(E9-I9))</f>
@@ -6806,25 +7895,25 @@
         <v/>
       </c>
       <c r="N9" s="185" t="n">
-        <v>112.18</v>
+        <v>114.46</v>
       </c>
       <c r="O9" s="35">
         <f>I9-J9</f>
         <v/>
       </c>
       <c r="P9" s="28" t="n">
-        <v>853.45</v>
+        <v>522.5</v>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S9" t="n">
-        <v>14387</v>
+        <v>24364</v>
       </c>
       <c r="T9" t="n">
-        <v>16608</v>
+        <v>25349</v>
       </c>
     </row>
     <row r="10">
@@ -6835,12 +7924,12 @@
       </c>
       <c r="B10" s="56" t="inlineStr">
         <is>
-          <t>27/05/2025</t>
+          <t>28/05/2025</t>
         </is>
       </c>
       <c r="C10" s="76" t="inlineStr">
         <is>
-          <t>25/06/2025</t>
+          <t>26/06/2025</t>
         </is>
       </c>
       <c r="D10" s="35">
@@ -6854,13 +7943,13 @@
       </c>
       <c r="H10" s="186" t="n"/>
       <c r="I10" s="28" t="n">
-        <v>1</v>
+        <v>678</v>
       </c>
       <c r="J10" s="28" t="n">
-        <v>1218</v>
+        <v>519</v>
       </c>
       <c r="K10" s="28" t="n">
-        <v>1318</v>
+        <v>619</v>
       </c>
       <c r="L10" s="75">
         <f>(K10+(E10-I10))</f>
@@ -6871,25 +7960,25 @@
         <v/>
       </c>
       <c r="N10" s="185" t="n">
-        <v>115.1</v>
+        <v>117.28</v>
       </c>
       <c r="O10" s="35">
         <f>I10-J10</f>
         <v/>
       </c>
       <c r="P10" s="28" t="n">
-        <v>752.25</v>
+        <v>627.5</v>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S10" t="n">
-        <v>16608</v>
+        <v>25349</v>
       </c>
       <c r="T10" t="n">
-        <v>17926</v>
+        <v>25968</v>
       </c>
     </row>
     <row r="11">
@@ -6900,12 +7989,12 @@
       </c>
       <c r="B11" s="56" t="inlineStr">
         <is>
-          <t>25/06/2025</t>
+          <t>26/06/2025</t>
         </is>
       </c>
       <c r="C11" s="76" t="inlineStr">
         <is>
-          <t>24/07/2025</t>
+          <t>25/07/2025</t>
         </is>
       </c>
       <c r="D11" s="35">
@@ -6919,13 +8008,13 @@
       </c>
       <c r="H11" s="186" t="n"/>
       <c r="I11" s="28" t="n">
-        <v>1</v>
+        <v>694</v>
       </c>
       <c r="J11" s="28" t="n">
-        <v>792</v>
+        <v>420</v>
       </c>
       <c r="K11" s="28" t="n">
-        <v>892</v>
+        <v>520</v>
       </c>
       <c r="L11" s="75">
         <f>(K11+(E11-I11))</f>
@@ -6936,25 +8025,25 @@
         <v/>
       </c>
       <c r="N11" s="185" t="n">
-        <v>115.11</v>
+        <v>117.27</v>
       </c>
       <c r="O11" s="35">
         <f>I11-J11</f>
         <v/>
       </c>
       <c r="P11" s="28" t="n">
-        <v>943.45</v>
+        <v>656</v>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S11" t="n">
-        <v>17926</v>
+        <v>25968</v>
       </c>
       <c r="T11" t="n">
-        <v>18818</v>
+        <v>26488</v>
       </c>
     </row>
     <row r="12">
@@ -6965,12 +8054,12 @@
       </c>
       <c r="B12" s="56" t="inlineStr">
         <is>
-          <t>24/07/2025</t>
+          <t>25/07/2025</t>
         </is>
       </c>
       <c r="C12" s="76" t="inlineStr">
         <is>
-          <t>25/08/2025</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="D12" s="35">
@@ -6984,13 +8073,13 @@
       </c>
       <c r="H12" s="186" t="n"/>
       <c r="I12" s="28" t="n">
-        <v>1</v>
+        <v>789</v>
       </c>
       <c r="J12" s="28" t="n">
-        <v>1559</v>
+        <v>535</v>
       </c>
       <c r="K12" s="28" t="n">
-        <v>1659</v>
+        <v>635</v>
       </c>
       <c r="L12" s="75">
         <f>(K12+(E12-I12))</f>
@@ -7001,25 +8090,25 @@
         <v/>
       </c>
       <c r="N12" s="185" t="n">
-        <v>115.88</v>
+        <v>118.33</v>
       </c>
       <c r="O12" s="35">
         <f>I12-J12</f>
         <v/>
       </c>
       <c r="P12" s="28" t="n">
-        <v>312.45</v>
+        <v>656</v>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S12" t="n">
-        <v>18818</v>
+        <v>26488</v>
       </c>
       <c r="T12" t="n">
-        <v>20477</v>
+        <v>27123</v>
       </c>
     </row>
     <row r="13">
@@ -7030,12 +8119,12 @@
       </c>
       <c r="B13" s="56" t="inlineStr">
         <is>
-          <t>25/08/2025</t>
+          <t>26/08/2025</t>
         </is>
       </c>
       <c r="C13" s="76" t="inlineStr">
         <is>
-          <t>23/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="D13" s="35">
@@ -7049,13 +8138,13 @@
       </c>
       <c r="H13" s="186" t="n"/>
       <c r="I13" s="28" t="n">
-        <v>1</v>
+        <v>1163</v>
       </c>
       <c r="J13" s="28" t="n">
-        <v>1294.85</v>
+        <v>701</v>
       </c>
       <c r="K13" s="28" t="n">
-        <v>1465</v>
+        <v>801</v>
       </c>
       <c r="L13" s="75">
         <f>(K13+(E13-I13))</f>
@@ -7066,25 +8155,25 @@
         <v/>
       </c>
       <c r="N13" s="185" t="n">
-        <v>195.09</v>
+        <v>120.32</v>
       </c>
       <c r="O13" s="35">
         <f>I13-J13</f>
         <v/>
       </c>
       <c r="P13" s="28" t="n">
-        <v>0</v>
+        <v>656</v>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S13" t="n">
-        <v>20477</v>
+        <v>27123</v>
       </c>
       <c r="T13" t="n">
-        <v>21942</v>
+        <v>27924</v>
       </c>
     </row>
     <row r="14">
@@ -7095,12 +8184,12 @@
       </c>
       <c r="B14" s="56" t="inlineStr">
         <is>
-          <t>23/09/2025</t>
+          <t>25/09/2025</t>
         </is>
       </c>
       <c r="C14" s="76" t="inlineStr">
         <is>
-          <t>25/10/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="D14" s="35">
@@ -7114,13 +8203,13 @@
       </c>
       <c r="H14" s="186" t="n"/>
       <c r="I14" s="28" t="n">
-        <v>1</v>
+        <v>597</v>
       </c>
       <c r="J14" s="28" t="n">
-        <v>1250.4</v>
+        <v>911</v>
       </c>
       <c r="K14" s="28" t="n">
-        <v>1662</v>
+        <v>1011</v>
       </c>
       <c r="L14" s="75">
         <f>(K14+(E14-I14))</f>
@@ -7131,25 +8220,25 @@
         <v/>
       </c>
       <c r="N14" s="185" t="n">
-        <v>471.11</v>
+        <v>127.31</v>
       </c>
       <c r="O14" s="35">
         <f>I14-J14</f>
         <v/>
       </c>
       <c r="P14" s="28" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S14" t="n">
-        <v>21942</v>
+        <v>27924</v>
       </c>
       <c r="T14" t="n">
-        <v>23604</v>
+        <v>28935</v>
       </c>
     </row>
     <row r="15">
@@ -7160,12 +8249,12 @@
       </c>
       <c r="B15" s="56" t="inlineStr">
         <is>
-          <t>25/10/2025</t>
+          <t>27/10/2025</t>
         </is>
       </c>
       <c r="C15" s="76" t="inlineStr">
         <is>
-          <t>25/11/2025</t>
+          <t>26/11/2025</t>
         </is>
       </c>
       <c r="D15" s="35">
@@ -7179,13 +8268,13 @@
       </c>
       <c r="H15" s="186" t="n"/>
       <c r="I15" s="28" t="n">
-        <v>0</v>
+        <v>919</v>
       </c>
       <c r="J15" s="28" t="n">
-        <v>403.2</v>
+        <v>651</v>
       </c>
       <c r="K15" s="28" t="n">
-        <v>1015</v>
+        <v>751</v>
       </c>
       <c r="L15" s="75">
         <f>(K15+(E15-I15))</f>
@@ -7196,25 +8285,25 @@
         <v/>
       </c>
       <c r="N15" s="185" t="n">
-        <v>793.74</v>
+        <v>145.54</v>
       </c>
       <c r="O15" s="35">
         <f>I15-J15</f>
         <v/>
       </c>
       <c r="P15" s="28" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>12932377-2</t>
+          <t>13168154-1</t>
         </is>
       </c>
       <c r="S15" t="n">
-        <v>23604</v>
+        <v>28935</v>
       </c>
       <c r="T15" t="n">
-        <v>24619</v>
+        <v>29686</v>
       </c>
     </row>
     <row r="16">
@@ -7223,11 +8312,16 @@
           <t>Dez</t>
         </is>
       </c>
-      <c r="B16" s="56">
-        <f>C15</f>
-        <v/>
-      </c>
-      <c r="C16" s="76" t="n"/>
+      <c r="B16" s="56" t="inlineStr">
+        <is>
+          <t>26/11/2025</t>
+        </is>
+      </c>
+      <c r="C16" s="76" t="inlineStr">
+        <is>
+          <t>27/12/2025</t>
+        </is>
+      </c>
       <c r="D16" s="35">
         <f>'RESUMO '!B25</f>
         <v/>
@@ -7238,9 +8332,15 @@
         <v/>
       </c>
       <c r="H16" s="166" t="n"/>
-      <c r="I16" s="28" t="n"/>
-      <c r="J16" s="28" t="n"/>
-      <c r="K16" s="28" t="n"/>
+      <c r="I16" s="28" t="n">
+        <v>808</v>
+      </c>
+      <c r="J16" s="28" t="n">
+        <v>748</v>
+      </c>
+      <c r="K16" s="28" t="n">
+        <v>848</v>
+      </c>
       <c r="L16" s="75">
         <f>(K16+(E16-I16))</f>
         <v/>
@@ -7249,12 +8349,27 @@
         <f>IFERROR(L16/$H$5,"")</f>
         <v/>
       </c>
-      <c r="N16" s="185" t="n"/>
+      <c r="N16" s="185" t="n">
+        <v>139.87</v>
+      </c>
       <c r="O16" s="35">
         <f>I16-J16</f>
         <v/>
       </c>
-      <c r="P16" s="28" t="n"/>
+      <c r="P16" s="28" t="n">
+        <v>342</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>13168154-1</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>29686</v>
+      </c>
+      <c r="T16" t="n">
+        <v>30534</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="32" t="inlineStr">
@@ -8057,30 +9172,30 @@
       </c>
       <c r="B16" s="56" t="inlineStr">
         <is>
-          <t>06/11/2025</t>
+          <t>21/11/2025</t>
         </is>
       </c>
       <c r="C16" s="76" t="inlineStr">
         <is>
-          <t>09/12/2025</t>
+          <t>22/12/2025</t>
         </is>
       </c>
       <c r="E16" s="166" t="n"/>
       <c r="F16" s="27" t="n">
-        <v>195</v>
+        <v>868</v>
       </c>
       <c r="G16" s="45">
         <f>IFERROR(F16/$E$5,"")</f>
         <v/>
       </c>
       <c r="H16" s="27" t="n">
-        <v>165</v>
+        <v>268</v>
       </c>
       <c r="I16" s="37" t="n">
         <v>0</v>
       </c>
       <c r="J16" s="185" t="n">
-        <v>40.29</v>
+        <v>763.62</v>
       </c>
       <c r="K16" s="48">
         <f>H16-F16</f>
@@ -8103,18 +9218,18 @@
         <v/>
       </c>
       <c r="Q16" s="28" t="n">
-        <v>28.97</v>
+        <v>0</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>10552579-1</t>
+          <t>2968374-2</t>
         </is>
       </c>
       <c r="T16" t="n">
-        <v>23883</v>
+        <v>93517</v>
       </c>
       <c r="U16" t="n">
-        <v>24078</v>
+        <v>94385</v>
       </c>
     </row>
     <row r="17">

</xml_diff>